<commit_message>
fixed some wrong digikey numbers
</commit_message>
<xml_diff>
--- a/hardware/nucleum/rev_a/nucleum_bom.xlsx
+++ b/hardware/nucleum/rev_a/nucleum_bom.xlsx
@@ -5,406 +5,411 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="141" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
+  <extLst>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="130">
   <si>
-    <t>Qty</t>
-  </si>
-  <si>
-    <t>Part</t>
-  </si>
-  <si>
-    <t>Value</t>
-  </si>
-  <si>
-    <t>Device</t>
-  </si>
-  <si>
-    <t>Package</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>DIGIKEY</t>
-  </si>
-  <si>
-    <t>MOUSER</t>
-  </si>
-  <si>
-    <t>NEWARK</t>
-  </si>
-  <si>
-    <t>RICHARDSON_RFPD</t>
-  </si>
-  <si>
-    <t>A1</t>
-  </si>
-  <si>
-    <t>FRACTUS-2.4GHZ-FR05-S1-N-0-102</t>
-  </si>
-  <si>
-    <t>FRACTUS-ANTENNA-FR05-S1-N-0-102</t>
-  </si>
-  <si>
-    <t>Fractus Compact Reach XtendTM chip antenna</t>
-  </si>
-  <si>
-    <t>FR05-S1-N-0102B</t>
-  </si>
-  <si>
-    <t>B1</t>
-  </si>
-  <si>
-    <t>BAL-NRF01D3</t>
-  </si>
-  <si>
-    <t>50 ohm nominal match balun to nRF51422-QFAA,</t>
-  </si>
-  <si>
-    <t>497-13637-1-ND</t>
-  </si>
-  <si>
-    <t>511-BAL-NRF01D3</t>
-  </si>
-  <si>
-    <t>DNP</t>
-  </si>
-  <si>
-    <t>ML-1220/F1AN</t>
-  </si>
-  <si>
-    <t>ML-1220/F1BN</t>
-  </si>
-  <si>
-    <t>BATTERY LITH 3V RECHARGE PC PINS</t>
-  </si>
-  <si>
-    <t>P663-nd</t>
-  </si>
-  <si>
-    <t>658-ML-1220/F1BN</t>
-  </si>
-  <si>
-    <t>C1</t>
-  </si>
-  <si>
-    <t>0.8pF</t>
-  </si>
-  <si>
-    <t>CAPACITOR</t>
-  </si>
-  <si>
-    <t>0402_CAP</t>
-  </si>
-  <si>
-    <t>0402 Capacitor</t>
-  </si>
-  <si>
-    <t>445-6269-1-ND</t>
-  </si>
-  <si>
-    <t>C2, C3, C4, C5</t>
-  </si>
-  <si>
-    <t>12pF</t>
-  </si>
-  <si>
-    <t>445-6197-1-ND</t>
-  </si>
-  <si>
-    <t>C6, C7</t>
-  </si>
-  <si>
-    <t>1nF</t>
-  </si>
-  <si>
-    <t>445-1303-1-ND</t>
-  </si>
-  <si>
-    <t>C8</t>
-  </si>
-  <si>
-    <t>2.2nF</t>
-  </si>
-  <si>
-    <t>445-5419-1-ND</t>
-  </si>
-  <si>
-    <t>C9</t>
-  </si>
-  <si>
-    <t>10nF</t>
-  </si>
-  <si>
-    <t>445-1260-1-ND</t>
-  </si>
-  <si>
-    <t>C10</t>
-  </si>
-  <si>
-    <t>47nF</t>
-  </si>
-  <si>
-    <t>445-1264-1-ND</t>
-  </si>
-  <si>
-    <t>C11, C12</t>
-  </si>
-  <si>
-    <t>0.1uF</t>
-  </si>
-  <si>
-    <t>445-1265-1-ND</t>
-  </si>
-  <si>
-    <t>C13</t>
-  </si>
-  <si>
-    <t>1uF</t>
-  </si>
-  <si>
-    <t>445-4998-1-ND</t>
-  </si>
-  <si>
-    <t>C14</t>
-  </si>
-  <si>
-    <t>4.7uF</t>
-  </si>
-  <si>
-    <t>445-5947-1-ND</t>
-  </si>
-  <si>
-    <t>10uF</t>
-  </si>
-  <si>
-    <t>CAPACITOR0603_CAP</t>
-  </si>
-  <si>
-    <t>0603_CAP</t>
-  </si>
-  <si>
-    <t>490-7316-1-ND</t>
-  </si>
-  <si>
-    <t>D1</t>
-  </si>
-  <si>
-    <t>SML-LX0404SIUPGUSB</t>
-  </si>
-  <si>
-    <t>1MM_SQ_4PAD</t>
-  </si>
-  <si>
-    <t>1mm^2 RGB LED</t>
-  </si>
-  <si>
-    <t>67-2125-1-ND</t>
-  </si>
-  <si>
-    <t>SH_MALE_2/1MM</t>
-  </si>
-  <si>
-    <t>SH-1X2/1MM</t>
-  </si>
-  <si>
-    <t>1.0mm pitch/Disconnectable Crimp style connectors</t>
-  </si>
-  <si>
-    <t>L1</t>
-  </si>
-  <si>
-    <t>15nH</t>
-  </si>
-  <si>
-    <t>INDUCTOR0402</t>
-  </si>
-  <si>
-    <t>0402_IND</t>
-  </si>
-  <si>
-    <t>0402 Inductor</t>
-  </si>
-  <si>
-    <t>587-1521-1-ND</t>
-  </si>
-  <si>
-    <t>2.2uH</t>
-  </si>
-  <si>
-    <t>INDUCTOR0603</t>
-  </si>
-  <si>
-    <t>0603_IND</t>
-  </si>
-  <si>
-    <t>FDK Multi-layer Power Inductor : MIPSZ2012D series (Very Small Type)</t>
-  </si>
-  <si>
-    <t>L3</t>
-  </si>
-  <si>
-    <t>10uH</t>
-  </si>
-  <si>
-    <t>0603 Inductor</t>
-  </si>
-  <si>
-    <t>490-4025-1-ND</t>
-  </si>
-  <si>
-    <t>R1, R2, R3</t>
-  </si>
-  <si>
-    <t>1k</t>
-  </si>
-  <si>
-    <t>RESISTOR0402_RES</t>
-  </si>
-  <si>
-    <t>0402_RES</t>
-  </si>
-  <si>
-    <t>Resistor</t>
-  </si>
-  <si>
-    <t>RHM1.0KCECT-ND</t>
-  </si>
-  <si>
-    <t>R4, R5</t>
-  </si>
-  <si>
-    <t>10k</t>
-  </si>
-  <si>
-    <t>RHM10KCECT-ND</t>
-  </si>
-  <si>
-    <t>R6</t>
-  </si>
-  <si>
-    <t>12k</t>
-  </si>
-  <si>
-    <t>RHM12.0KCDCT-ND</t>
-  </si>
-  <si>
-    <t>RES_SWITCH-0k</t>
-  </si>
-  <si>
-    <t>RES_SWITCH</t>
-  </si>
-  <si>
-    <t>0402 Static Resistor Selector</t>
-  </si>
-  <si>
-    <t>U2</t>
-  </si>
-  <si>
-    <t>FM25LBTDFN-8</t>
-  </si>
-  <si>
-    <t>TDFN-8</t>
-  </si>
-  <si>
-    <t>IC FRAM 4KBIT 10MHZ 8SOIC</t>
-  </si>
-  <si>
-    <t>FM25L04B-DGRA-ND</t>
-  </si>
-  <si>
-    <t>877-FM25L04B-DG</t>
-  </si>
-  <si>
-    <t>U3</t>
-  </si>
-  <si>
-    <t>RV-3049-C3</t>
-  </si>
-  <si>
-    <t>MICRO-CRYSTAL-C3</t>
-  </si>
-  <si>
-    <t>The RV-3049-C3 is an ultra miniature Real-Time-Clock Module</t>
-  </si>
-  <si>
-    <t>09X0513</t>
-  </si>
-  <si>
-    <t>TPS62740</t>
-  </si>
-  <si>
-    <t>R-PWSON-12</t>
-  </si>
-  <si>
-    <t>360nA Step Down Converter for Low Power Applications</t>
-  </si>
-  <si>
-    <t>296-37134-1-ND</t>
-  </si>
-  <si>
-    <t>595-TPS62740DSST</t>
-  </si>
-  <si>
-    <t>27X9745</t>
-  </si>
-  <si>
-    <t>U5</t>
-  </si>
-  <si>
-    <t>NRF51822QF</t>
-  </si>
-  <si>
-    <t>QFN-48-6MM</t>
-  </si>
-  <si>
-    <t>Multiprotocol Bluetooth® 4.0 low energy/2.4 GHz RF SoC</t>
-  </si>
-  <si>
-    <t>1490-1040-1-ND</t>
-  </si>
-  <si>
-    <t>949-NRF51822-QFAB-R7</t>
-  </si>
-  <si>
-    <t>X1</t>
-  </si>
-  <si>
-    <t>16MHz</t>
-  </si>
-  <si>
-    <t>TXC-8Y</t>
-  </si>
-  <si>
-    <t>CRYSTAL 16MHZ 8PF SMD</t>
-  </si>
-  <si>
-    <t>887-2003-1-ND</t>
-  </si>
-  <si>
-    <t>X2</t>
-  </si>
-  <si>
-    <t>ABS05-32.768KHZ-T</t>
-  </si>
-  <si>
-    <t>ABS05</t>
-  </si>
-  <si>
-    <t>32.768kHz Crystal</t>
-  </si>
-  <si>
-    <t>535-11899-1-ND</t>
+    <t xml:space="preserve">Qty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Part</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Device</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Package</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DIGIKEY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MOUSER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NEWARK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RICHARDSON_RFPD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FRACTUS-2.4GHZ-FR05-S1-N-0-102</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FRACTUS-ANTENNA-FR05-S1-N-0-102</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fractus Compact Reach XtendTM chip antenna</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FR05-S1-N-0102B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BAL-NRF01D3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">50 ohm nominal match balun to nRF51422-QFAA,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">497-13637-1-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">511-BAL-NRF01D3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DNP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ML-1220/F1AN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ML-1220/F1BN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BATTERY LITH 3V RECHARGE PC PINS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P663-nd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">658-ML-1220/F1BN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.8pF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAPACITOR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0402_CAP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0402 Capacitor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">490-6269-1-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C2, C3, C4, C5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12pF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">490-6197-1-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C6, C7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1nF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">490-1303-1-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.2nF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">490-5419-1-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10nF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">445-1260-1-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">47nF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">445-1264-1-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C11, C12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.1uF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">445-1265-1-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1uF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">445-4998-1-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4.7uF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">445-5947-1-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10uF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAPACITOR0603_CAP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0603_CAP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">490-7316-1-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SML-LX0404SIUPGUSB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1MM_SQ_4PAD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1mm^2 RGB LED</t>
+  </si>
+  <si>
+    <t xml:space="preserve">67-2125-1-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SH_MALE_2/1MM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SH-1X2/1MM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.0mm pitch/Disconnectable Crimp style connectors</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15nH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INDUCTOR0402</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0402_IND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0402 Inductor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">587-1521-1-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.2uH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INDUCTOR0603</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0603_IND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FDK Multi-layer Power Inductor : MIPSZ2012D series (Very Small Type)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10uH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0603 Inductor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">490-4025-1-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R1, R2, R3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1k</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESISTOR0402_RES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0402_RES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resistor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RHM1.0KCECT-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R4, R5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10k</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RHM10KCECT-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12k</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RHM12.0KCDCT-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RES_SWITCH-0k</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RES_SWITCH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0402 Static Resistor Selector</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FM25LBTDFN-8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TDFN-8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IC FRAM 4KBIT 10MHZ 8SOIC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FM25L04B-DGRA-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">877-FM25L04B-DG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RV-3049-C3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MICRO-CRYSTAL-C3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The RV-3049-C3 is an ultra miniature Real-Time-Clock Module</t>
+  </si>
+  <si>
+    <t xml:space="preserve">09X0513</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TPS62740</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R-PWSON-12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">360nA Step Down Converter for Low Power Applications</t>
+  </si>
+  <si>
+    <t xml:space="preserve">296-37134-1-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">595-TPS62740DSST</t>
+  </si>
+  <si>
+    <t xml:space="preserve">27X9745</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NRF51822QF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">QFN-48-6MM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Multiprotocol Bluetooth® 4.0 low energy/2.4 GHz RF SoC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1490-1040-1-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">949-NRF51822-QFAB-R7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">X1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16MHz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TXC-8Y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CRYSTAL 16MHZ 8PF SMD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">887-2003-1-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">X2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ABS05-32.768KHZ-T</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ABS05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">32.768kHz Crystal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">535-11899-1-ND</t>
   </si>
 </sst>
 </file>
@@ -412,7 +417,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -527,22 +532,22 @@
   <dimension ref="A1:J29"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F25" activeCellId="0" sqref="F25"/>
+      <selection pane="topLeft" activeCell="G29" activeCellId="0" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="4.99489795918367"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.7959183673469"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.3928571428571"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="31.3010204081633"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="33.6683673469388"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="59.7857142857143"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.0765306122449"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="21.7142857142857"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.65816326530612"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="19.3571428571429"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="4.86224489795918"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.6326530612245"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.1938775510204"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.9132653061224"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="33.3418367346939"/>
+    <col collapsed="false" hidden="true" max="6" min="6" style="0" width="0"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.8979591836735"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="21.4642857142857"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="19.0357142857143"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>